<commit_message>
Added some test cases
</commit_message>
<xml_diff>
--- a/documentation/sprint 3/Sprint 3 Tests.xlsx
+++ b/documentation/sprint 3/Sprint 3 Tests.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4518DE0-B448-403B-A10A-E339989F0C78}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{705768B7-CE72-495F-A5CD-3AB1A416A85E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
   <si>
     <t>Test</t>
   </si>
@@ -74,6 +74,69 @@
   </si>
   <si>
     <t>deleted javaScript and added if statements</t>
+  </si>
+  <si>
+    <t>displayed home page</t>
+  </si>
+  <si>
+    <t>IO File Not Found error</t>
+  </si>
+  <si>
+    <t>transferred statics files to AWS</t>
+  </si>
+  <si>
+    <t>Read CSV from S3 bucket</t>
+  </si>
+  <si>
+    <t>Deploying to Heroku</t>
+  </si>
+  <si>
+    <t>Properly Formatted Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> All the data in one string</t>
+  </si>
+  <si>
+    <t>Imported Boto3 and read files using that</t>
+  </si>
+  <si>
+    <t>Deploying to Heroku V2</t>
+  </si>
+  <si>
+    <t>Import Error Module win32timezone not found</t>
+  </si>
+  <si>
+    <t>Removed unnecessary imports</t>
+  </si>
+  <si>
+    <t>Generate Bracket for 2015</t>
+  </si>
+  <si>
+    <t>Ordered list of winners of each round</t>
+  </si>
+  <si>
+    <t>Out of Bounds Exceptions for seeds</t>
+  </si>
+  <si>
+    <t>Imported urllib2 and read seeds with url.open</t>
+  </si>
+  <si>
+    <t>Generate Bracket for 2018</t>
+  </si>
+  <si>
+    <t>Still Broken, needs fix</t>
+  </si>
+  <si>
+    <t>Display Indicators on Home page</t>
+  </si>
+  <si>
+    <t>Formatted in a table like structure</t>
+  </si>
+  <si>
+    <t>All in one big string</t>
+  </si>
+  <si>
+    <t>added paragraph markers and breaks</t>
   </si>
 </sst>
 </file>
@@ -411,22 +474,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="37.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.7890625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.3125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.7890625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -443,7 +506,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -460,7 +523,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -477,7 +540,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -491,6 +554,108 @@
         <v>15</v>
       </c>
       <c r="E4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added dates to tests
</commit_message>
<xml_diff>
--- a/documentation/sprint 3/Sprint 3 Tests.xlsx
+++ b/documentation/sprint 3/Sprint 3 Tests.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F0D19AF-914C-43A9-9948-43D82397B541}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{775E9BEF-784F-4E64-9056-E80B49962076}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="83">
   <si>
     <t>Test</t>
   </si>
@@ -322,9 +322,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -608,7 +610,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D3" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -616,7 +620,7 @@
     <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.3125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.7890625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.15625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.75">
@@ -649,8 +653,8 @@
       <c r="D2" t="s">
         <v>16</v>
       </c>
-      <c r="E2" t="s">
-        <v>15</v>
+      <c r="E2" s="2">
+        <v>43195</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -666,8 +670,8 @@
       <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
-        <v>15</v>
+      <c r="E3" s="2">
+        <v>43195</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -700,8 +704,8 @@
       <c r="D5" t="s">
         <v>74</v>
       </c>
-      <c r="E5" t="s">
-        <v>15</v>
+      <c r="E5" s="3">
+        <v>43197</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -717,8 +721,8 @@
       <c r="D6" t="s">
         <v>82</v>
       </c>
-      <c r="E6" t="s">
-        <v>15</v>
+      <c r="E6" s="3">
+        <v>43197</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -734,8 +738,8 @@
       <c r="D7" t="s">
         <v>19</v>
       </c>
-      <c r="E7" t="s">
-        <v>15</v>
+      <c r="E7" s="3">
+        <v>43197</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -751,8 +755,8 @@
       <c r="D8" t="s">
         <v>24</v>
       </c>
-      <c r="E8" t="s">
-        <v>15</v>
+      <c r="E8" s="3">
+        <v>43205</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -768,8 +772,8 @@
       <c r="D9" t="s">
         <v>27</v>
       </c>
-      <c r="E9" t="s">
-        <v>15</v>
+      <c r="E9" s="3">
+        <v>43205</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -785,8 +789,8 @@
       <c r="D10" t="s">
         <v>31</v>
       </c>
-      <c r="E10" t="s">
-        <v>15</v>
+      <c r="E10" s="3">
+        <v>43205</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -819,8 +823,8 @@
       <c r="D12" t="s">
         <v>37</v>
       </c>
-      <c r="E12" t="s">
-        <v>15</v>
+      <c r="E12" s="3">
+        <v>43206</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -836,8 +840,8 @@
       <c r="D13" t="s">
         <v>41</v>
       </c>
-      <c r="E13" t="s">
-        <v>15</v>
+      <c r="E13" s="3">
+        <v>43206</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -853,8 +857,8 @@
       <c r="D14" t="s">
         <v>45</v>
       </c>
-      <c r="E14" t="s">
-        <v>15</v>
+      <c r="E14" s="3">
+        <v>43205</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -870,8 +874,8 @@
       <c r="D15" t="s">
         <v>49</v>
       </c>
-      <c r="E15" t="s">
-        <v>15</v>
+      <c r="E15" s="3">
+        <v>43204</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -887,8 +891,8 @@
       <c r="D16" t="s">
         <v>53</v>
       </c>
-      <c r="E16" t="s">
-        <v>15</v>
+      <c r="E16" s="3">
+        <v>43203</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -904,8 +908,8 @@
       <c r="D17" t="s">
         <v>57</v>
       </c>
-      <c r="E17" t="s">
-        <v>15</v>
+      <c r="E17" s="3">
+        <v>43203</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -921,8 +925,8 @@
       <c r="D18" t="s">
         <v>61</v>
       </c>
-      <c r="E18" t="s">
-        <v>15</v>
+      <c r="E18" s="3">
+        <v>43204</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -938,8 +942,8 @@
       <c r="D19" t="s">
         <v>78</v>
       </c>
-      <c r="E19" t="s">
-        <v>15</v>
+      <c r="E19" s="3">
+        <v>43200</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -955,8 +959,8 @@
       <c r="D20" t="s">
         <v>65</v>
       </c>
-      <c r="E20" t="s">
-        <v>15</v>
+      <c r="E20" s="3">
+        <v>43204</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -972,8 +976,8 @@
       <c r="D21" t="s">
         <v>69</v>
       </c>
-      <c r="E21" t="s">
-        <v>15</v>
+      <c r="E21" s="3">
+        <v>43204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>